<commit_message>
added decision tree notes
</commit_message>
<xml_diff>
--- a/Machine Learning/Classification Models/Decision Tree/Gini gain explaination sheet.xlsx
+++ b/Machine Learning/Classification Models/Decision Tree/Gini gain explaination sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Class_Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Class_Notes\Machine Learning\Classification Models\Decision Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CBF7E78B-717E-42C8-81A6-A98B95EF1C35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B251DF-40EF-4496-BAF0-5514A6C31E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{5D836753-1546-4A9B-AE48-5488417F41B1}"/>
   </bookViews>
@@ -22,12 +22,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="54">
   <si>
     <t>Gender</t>
   </si>
@@ -173,13 +182,39 @@
   </si>
   <si>
     <t>So here the gini gain of age is greater than gender and region so here the split happened by  age</t>
+  </si>
+  <si>
+    <t>Note:= Decision tree not only take 25 it will test with all and e.g &lt;23 &gt;28 etc and take that which is best.</t>
+  </si>
+  <si>
+    <t>We will try with age&lt;23</t>
+  </si>
+  <si>
+    <t>Age&lt;23
+N:1        Target:0</t>
+  </si>
+  <si>
+    <t>Age&gt;=23
+N:9      Target:4</t>
+  </si>
+  <si>
+    <t>1-((0/1)^2+(1/1)^2)</t>
+  </si>
+  <si>
+    <t>1-((4/9)^2+(5/9)^2)</t>
+  </si>
+  <si>
+    <t>(1/10)*0+(9/10)*0.49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">here we see 0.039 is less than 0.48 which is come at age&lt;25 case so decision tree algorithm try with every age and find the best which has large gini index. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,6 +250,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -291,21 +333,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -315,7 +358,15 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,6 +688,112 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5135880" y="739140"/>
+          <a:ext cx="769620" cy="541020"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F78965AF-F6A6-48C0-A91A-D14FF0C8CACF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3779520" y="716280"/>
+          <a:ext cx="647700" cy="579120"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E74297D1-0A98-4560-9E17-C3A44AFF5394}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4640580" y="739140"/>
           <a:ext cx="769620" cy="541020"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -1005,13 +1162,13 @@
       <c r="D2" s="2">
         <v>0</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1028,12 +1185,12 @@
       <c r="D3" s="2">
         <v>1</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="L3" s="7" t="s">
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="L3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="M3" s="2" t="s">
@@ -1056,10 +1213,10 @@
       <c r="D4" s="2">
         <v>1</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="L4" s="7" t="s">
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="L4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="M4" s="2" t="s">
@@ -1082,7 +1239,7 @@
       <c r="D5" s="2">
         <v>0</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="M5" s="2" t="s">
@@ -1105,7 +1262,7 @@
       <c r="D6" s="2">
         <v>1</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="L6" s="4" t="s">
         <v>17</v>
       </c>
       <c r="M6" s="2" t="s">
@@ -1128,7 +1285,7 @@
       <c r="D7" s="2">
         <v>0</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="L7" s="4" t="s">
         <v>18</v>
       </c>
       <c r="M7" s="2" t="s">
@@ -1151,14 +1308,14 @@
       <c r="D8" s="2">
         <v>0</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="5"/>
-      <c r="I8" s="4" t="s">
+      <c r="G8" s="7"/>
+      <c r="I8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="5"/>
+      <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -1173,10 +1330,10 @@
       <c r="D9" s="2">
         <v>0</v>
       </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -1207,32 +1364,32 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
     </row>
     <row r="15" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
     </row>
     <row r="16" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F16" s="10"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1289,13 +1446,13 @@
       <c r="D2" s="2">
         <v>0</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1312,12 +1469,12 @@
       <c r="D3" s="2">
         <v>1</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="L3" s="7" t="s">
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="L3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="M3" s="2" t="s">
@@ -1341,10 +1498,10 @@
       <c r="D4" s="2">
         <v>1</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="L4" s="7" t="s">
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="L4" s="4" t="s">
         <v>29</v>
       </c>
       <c r="M4" s="2" t="s">
@@ -1368,7 +1525,7 @@
       <c r="D5" s="2">
         <v>0</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="4" t="s">
         <v>30</v>
       </c>
       <c r="M5" s="2" t="s">
@@ -1392,7 +1549,7 @@
       <c r="D6" s="2">
         <v>1</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="L6" s="4" t="s">
         <v>31</v>
       </c>
       <c r="M6" s="2" t="s">
@@ -1416,7 +1573,7 @@
       <c r="D7" s="2">
         <v>0</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="L7" s="4" t="s">
         <v>18</v>
       </c>
       <c r="M7" s="2" t="s">
@@ -1440,14 +1597,14 @@
       <c r="D8" s="2">
         <v>0</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="5"/>
-      <c r="I8" s="4" t="s">
+      <c r="G8" s="7"/>
+      <c r="I8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="5"/>
+      <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -1462,10 +1619,10 @@
       <c r="D9" s="2">
         <v>0</v>
       </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -1496,32 +1653,32 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="F16" s="10"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1539,14 +1696,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA814901-EB7F-4806-A921-B5CD404A39D9}">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="11" max="11" width="17.5546875" customWidth="1"/>
     <col min="12" max="12" width="26.33203125" customWidth="1"/>
     <col min="13" max="13" width="27.77734375" customWidth="1"/>
   </cols>
@@ -1578,13 +1736,13 @@
       <c r="D2" s="2">
         <v>0</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1601,12 +1759,12 @@
       <c r="D3" s="2">
         <v>1</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="L3" s="7" t="s">
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="L3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="M3" s="2" t="s">
@@ -1629,10 +1787,10 @@
       <c r="D4" s="2">
         <v>1</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="L4" s="7" t="s">
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="L4" s="4" t="s">
         <v>37</v>
       </c>
       <c r="M4" s="2" t="s">
@@ -1656,7 +1814,7 @@
       <c r="D5" s="2">
         <v>0</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="4" t="s">
         <v>38</v>
       </c>
       <c r="M5" s="2" t="s">
@@ -1680,7 +1838,7 @@
       <c r="D6" s="2">
         <v>1</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="L6" s="4" t="s">
         <v>39</v>
       </c>
       <c r="M6" s="2" t="s">
@@ -1704,7 +1862,7 @@
       <c r="D7" s="2">
         <v>0</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="L7" s="4" t="s">
         <v>18</v>
       </c>
       <c r="M7" s="2" t="s">
@@ -1727,14 +1885,14 @@
       <c r="D8" s="2">
         <v>0</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="5"/>
-      <c r="I8" s="4" t="s">
+      <c r="G8" s="7"/>
+      <c r="I8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="J8" s="5"/>
+      <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -1749,10 +1907,10 @@
       <c r="D9" s="2">
         <v>0</v>
       </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -1783,47 +1941,50 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="F16" s="10"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F16" s="11"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="11" t="s">
+      <c r="E19" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>0</v>
       </c>
@@ -1831,7 +1992,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>1</v>
       </c>
@@ -1839,7 +2000,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
@@ -1847,21 +2008,140 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+    </row>
+    <row r="28" spans="1:13" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="E28" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F31" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="K31" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="K32" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M32" s="2">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="33" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="K33" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M33" s="2">
+        <f>1-((0/1)^2+(1/1)^2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="K34" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M34" s="14">
+        <f>1-((4/9)^2+(5/9)^2)</f>
+        <v>0.49382716049382713</v>
+      </c>
+    </row>
+    <row r="35" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="K35" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="M35" s="2">
+        <f>(1/10)*0+(9/10)*0.49</f>
+        <v>0.441</v>
+      </c>
+    </row>
+    <row r="36" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E36" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F36" s="7"/>
+      <c r="H36" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I36" s="7"/>
+      <c r="K36" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M36" s="2">
+        <f>0.48-0.441</f>
+        <v>3.8999999999999979E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+    </row>
+    <row r="39" spans="5:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K39" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="L39" s="15"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="16"/>
+    </row>
+    <row r="40" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="K40" s="15"/>
+      <c r="L40" s="15"/>
+      <c r="M40" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="12">
+    <mergeCell ref="K39:M40"/>
+    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="H36:I37"/>
+    <mergeCell ref="F31:H32"/>
+    <mergeCell ref="E36:F37"/>
     <mergeCell ref="A25:I25"/>
     <mergeCell ref="G3:I4"/>
     <mergeCell ref="F8:G9"/>

</xml_diff>